<commit_message>
MSP430 board: optimized pcb, updated leds with correct leds, double checked pcb. passed DRM. Besides that, added digikey and samtec order summaries.
</commit_message>
<xml_diff>
--- a/hardware/bom/MSP_BOM_Record.xlsx
+++ b/hardware/bom/MSP_BOM_Record.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="125">
   <si>
     <t>Part</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Capacitor 0.01uF</t>
   </si>
   <si>
-    <t>Capacitor 0.01uF -&gt; try 0.1uF</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 50V 10% X7R 1206</t>
   </si>
   <si>
@@ -186,18 +183,12 @@
     <t xml:space="preserve">Capacitor 0.1uF </t>
   </si>
   <si>
-    <t>SEE NEXT ROW</t>
-  </si>
-  <si>
     <t>SW-PB</t>
   </si>
   <si>
     <t>PUSH BUTTON SWITCH TACTILE SPST-NO 0.05A 24V</t>
   </si>
   <si>
-    <t>in-progress order 3</t>
-  </si>
-  <si>
     <t>Omran Electronics</t>
   </si>
   <si>
@@ -213,9 +204,6 @@
     <t>JTAG Header</t>
   </si>
   <si>
-    <t>in-progress order 2</t>
-  </si>
-  <si>
     <t>JTAG HEADER DOUBLE ROW HEADER, 5 PINS PER ROW</t>
   </si>
   <si>
@@ -228,18 +216,6 @@
     <t>LED, Red</t>
   </si>
   <si>
-    <t>LNJ308G8LRA</t>
-  </si>
-  <si>
-    <t>LNJ208R8ARA</t>
-  </si>
-  <si>
-    <t>Green LED</t>
-  </si>
-  <si>
-    <t>Red LED</t>
-  </si>
-  <si>
     <t>ERJ-8GEYJ301V</t>
   </si>
   <si>
@@ -351,9 +327,6 @@
     <t>in-progress order 10 (total 5)</t>
   </si>
   <si>
-    <t>in-progress order 2 (tota need 1)</t>
-  </si>
-  <si>
     <t>in-progress order 3 (total need 1)</t>
   </si>
   <si>
@@ -366,9 +339,6 @@
     <t>in-progress order 4 (total need 2)</t>
   </si>
   <si>
-    <t>in-progress order  6 (total need 4)</t>
-  </si>
-  <si>
     <t>in-hand (total need 2)</t>
   </si>
   <si>
@@ -376,6 +346,51 @@
   </si>
   <si>
     <t>in-progress order 3 (total need 2)</t>
+  </si>
+  <si>
+    <t>C1206C103J1RACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 100V 5% X7R 1206</t>
+  </si>
+  <si>
+    <t>in-progress order 5 (total need 2)</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>LTST-C230EKT</t>
+  </si>
+  <si>
+    <t>LED RED-ORAN CLR1206REAR MNT SMD</t>
+  </si>
+  <si>
+    <t>LED, Amber</t>
+  </si>
+  <si>
+    <t>LTST-C230AKT</t>
+  </si>
+  <si>
+    <t>LED AMBER CLR 1206 REAR MNT SMD</t>
+  </si>
+  <si>
+    <t>LTST-C150GKT</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 1206 SMD</t>
+  </si>
+  <si>
+    <t>Ribbon Cable</t>
+  </si>
+  <si>
+    <t>IDSS-03-D-04.00</t>
+  </si>
+  <si>
+    <t>CABLE ASSEMBLY FEMALE SINGLE ROW 3 PINS</t>
+  </si>
+  <si>
+    <t>IDMS-03-T-04.00-T</t>
   </si>
 </sst>
 </file>
@@ -391,16 +406,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -428,9 +442,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N53"/>
+  <dimension ref="A2:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J7" t="s">
         <v>38</v>
@@ -909,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J8" t="s">
         <v>38</v>
@@ -917,36 +931,57 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
       </c>
       <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
         <v>53</v>
       </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>54</v>
-      </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="J10" t="s">
         <v>38</v>
@@ -954,16 +989,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -975,30 +1010,30 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="J11" t="s">
         <v>38</v>
       </c>
       <c r="K11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
@@ -1010,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J12" t="s">
         <v>38</v>
@@ -1086,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="J19" t="s">
         <v>38</v>
@@ -1152,16 +1187,16 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -1173,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="J22" t="s">
         <v>38</v>
@@ -1181,16 +1216,16 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -1202,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="J23" t="s">
         <v>38</v>
@@ -1210,16 +1245,16 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -1231,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="H24" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J24" t="s">
         <v>38</v>
@@ -1239,28 +1274,28 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
       <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
         <v>53</v>
-      </c>
-      <c r="D25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" t="s">
-        <v>54</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="J25" t="s">
         <v>38</v>
@@ -1268,16 +1303,16 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -1289,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="J26" t="s">
         <v>38</v>
@@ -1299,19 +1334,43 @@
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>
@@ -1323,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="J28" t="s">
         <v>38</v>
@@ -1331,231 +1390,212 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
       </c>
       <c r="F29">
-        <v>0.46</v>
+        <v>0.4</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J29" t="s">
         <v>38</v>
-      </c>
-      <c r="K29" t="s">
-        <v>62</v>
-      </c>
-      <c r="L29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
       </c>
       <c r="F30">
-        <v>0.56000000000000005</v>
+        <v>0.4</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J30" t="s">
         <v>38</v>
       </c>
-      <c r="K30" t="s">
-        <v>62</v>
-      </c>
-      <c r="L30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>67</v>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31">
+        <v>0.38</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>106</v>
+      </c>
+      <c r="J31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>105</v>
+      </c>
+      <c r="J32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>40</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D39" t="s">
         <v>42</v>
       </c>
-      <c r="E37" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37">
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39">
         <v>0.36</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>108</v>
-      </c>
-      <c r="J37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38">
-        <v>0.46</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
-        <v>115</v>
-      </c>
-      <c r="J38" t="s">
-        <v>38</v>
-      </c>
-      <c r="K38" t="s">
-        <v>62</v>
-      </c>
-      <c r="L38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39">
-        <v>0.56000000000000005</v>
-      </c>
       <c r="G39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="J39" t="s">
         <v>38</v>
-      </c>
-      <c r="K39" t="s">
-        <v>62</v>
-      </c>
-      <c r="L39" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1567,7 +1607,7 @@
         <v>2</v>
       </c>
       <c r="H40" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J40" t="s">
         <v>38</v>
@@ -1575,19 +1615,19 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E41" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F41">
         <v>22.95</v>
@@ -1596,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I41">
         <v>2</v>
@@ -1605,226 +1645,322 @@
         <v>38</v>
       </c>
     </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42">
+        <v>0.4</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>106</v>
+      </c>
+      <c r="J42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43">
+        <v>0.4</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>106</v>
+      </c>
+      <c r="J43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44">
+        <v>0.38</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>106</v>
+      </c>
+      <c r="J44" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>45</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51">
+        <v>0.94</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>104</v>
+      </c>
+      <c r="J51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52">
+        <v>0.31</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52" t="s">
+        <v>109</v>
+      </c>
+      <c r="J52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53">
+        <v>0.36</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53" t="s">
+        <v>100</v>
+      </c>
+      <c r="J53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54">
+        <v>0.96</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>104</v>
+      </c>
+      <c r="J54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" t="s">
         <v>94</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D55" t="s">
         <v>95</v>
       </c>
-      <c r="D48" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48">
-        <v>0.94</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
-        <v>113</v>
-      </c>
-      <c r="J48" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="E55" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55" t="s">
+        <v>108</v>
+      </c>
+      <c r="J55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" t="s">
         <v>98</v>
       </c>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="D56" t="s">
+        <v>99</v>
+      </c>
+      <c r="E56" t="s">
         <v>97</v>
       </c>
-      <c r="E49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49">
-        <v>0.31</v>
-      </c>
-      <c r="G49">
+      <c r="F56" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56">
         <v>2</v>
       </c>
-      <c r="H49" t="s">
-        <v>119</v>
-      </c>
-      <c r="J49" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" t="s">
-        <v>41</v>
-      </c>
-      <c r="D50" t="s">
-        <v>42</v>
-      </c>
-      <c r="E50" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50">
-        <v>0.36</v>
-      </c>
-      <c r="G50">
-        <v>5</v>
-      </c>
-      <c r="H50" t="s">
-        <v>108</v>
-      </c>
-      <c r="J50" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" t="s">
-        <v>100</v>
-      </c>
-      <c r="E51" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51">
-        <v>0.96</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51" t="s">
-        <v>113</v>
-      </c>
-      <c r="J51" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" t="s">
-        <v>102</v>
-      </c>
-      <c r="D52" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" t="s">
-        <v>29</v>
-      </c>
-      <c r="G52">
-        <v>4</v>
-      </c>
-      <c r="H52" t="s">
-        <v>118</v>
-      </c>
-      <c r="J52" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>104</v>
-      </c>
-      <c r="B53" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" t="s">
-        <v>106</v>
-      </c>
-      <c r="D53" t="s">
-        <v>107</v>
-      </c>
-      <c r="E53" t="s">
-        <v>105</v>
-      </c>
-      <c r="F53" t="s">
-        <v>29</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53">
-        <v>2</v>
-      </c>
-      <c r="J53" t="s">
+      <c r="J56" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added documentation of MSP430 Board along with document for milestone 2 demo.
</commit_message>
<xml_diff>
--- a/hardware/bom/MSP_BOM_Record.xlsx
+++ b/hardware/bom/MSP_BOM_Record.xlsx
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>